<commit_message>
small changes to distribution
</commit_message>
<xml_diff>
--- a/distribution.xlsx
+++ b/distribution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas\Documents\GitHub\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62F332F4-4373-430B-A4D1-17BAE2C03101}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEABC0A-B6BD-40C5-ADF5-A729C368939F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -610,7 +610,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +964,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="1">
-        <v>43635</v>
+        <v>43637</v>
       </c>
       <c r="G7" s="6">
         <v>17</v>
@@ -1184,7 +1184,7 @@
         <v>12</v>
       </c>
       <c r="F11" s="1">
-        <v>43626</v>
+        <v>43630</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>32</v>
@@ -1514,7 +1514,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="1">
-        <v>43626</v>
+        <v>43628</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>32</v>

</xml_diff>